<commit_message>
Fix graduation rate: degree-specific lookback (4yr bach, 2yr master, 3yr PhD)
- Fixed graduation on-time calculation to use correct lookback period per degree
- Bachelor's: 4 years, Master's: 2 years, PhD: 3 years
- Display retained students as "X من Y" format (e.g., "24 من 30")
- Display on-time graduates as "X من Y" format (e.g., "10 من 11")
- Added detail text under KPI cards for graduation and retention rates
- Regenerated data.csv and Excel file with corrected calculations

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/KPI_Data_Complete.xlsx
+++ b/data/KPI_Data_Complete.xlsx
@@ -1273,7 +1273,7 @@
     </row>
     <row r="7" ht="35" customHeight="1">
       <c r="A7" s="5" t="n">
-        <v>0.6354929577464788</v>
+        <v>0.6071232876712329</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>0.8386123680241327</v>
@@ -1477,10 +1477,8 @@
       <c r="F15" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="17" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="G15" s="16" t="n">
+        <v>0.25</v>
       </c>
       <c r="H15" s="12" t="n">
         <v>1</v>
@@ -1510,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="12" t="n">
-        <v>0.8</v>
+        <v>0.71875</v>
       </c>
       <c r="H16" s="12" t="n">
         <v>0.9565217391304348</v>
@@ -1540,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="12" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="H17" s="12" t="n">
         <v>0.8809523809523809</v>
@@ -1569,10 +1567,8 @@
       <c r="F18" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="18" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="G18" s="16" t="n">
+        <v>0</v>
       </c>
       <c r="H18" s="12" t="n">
         <v>0.9285714285714286</v>
@@ -1601,10 +1597,8 @@
       <c r="F19" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="17" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="G19" s="16" t="n">
+        <v>0.3823529411764706</v>
       </c>
       <c r="H19" s="12" t="n">
         <v>1</v>
@@ -1633,10 +1627,8 @@
       <c r="F20" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="18" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="G20" s="15" t="n">
+        <v>0.6923076923076923</v>
       </c>
       <c r="H20" s="12" t="n">
         <v>0.8947368421052632</v>
@@ -1665,10 +1657,8 @@
       <c r="F21" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="17" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="G21" s="16" t="n">
+        <v>0.1176470588235294</v>
       </c>
       <c r="H21" s="12" t="n">
         <v>1</v>
@@ -1698,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="12" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H22" s="12" t="n">
         <v>0.8888888888888888</v>
@@ -1758,7 +1748,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="15" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="H24" s="12" t="n">
         <v>0.8181818181818182</v>
@@ -1788,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="12" t="n">
-        <v>0.7916666666666666</v>
+        <v>1</v>
       </c>
       <c r="H25" s="12" t="n">
         <v>0.9285714285714286</v>
@@ -1957,10 +1947,8 @@
       <c r="E33" s="14" t="n">
         <v>1947</v>
       </c>
-      <c r="F33" s="18" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="F33" s="18" t="n">
+        <v>0.5</v>
       </c>
       <c r="G33" s="18" t="n">
         <v>0.9579901153212521</v>
@@ -1987,10 +1975,8 @@
       <c r="E34" s="11" t="n">
         <v>1734</v>
       </c>
-      <c r="F34" s="17" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="F34" s="17" t="n">
+        <v>0.9272727272727272</v>
       </c>
       <c r="G34" s="17" t="n">
         <v>0.9313160422670509</v>
@@ -2018,7 +2004,7 @@
         <v>1299</v>
       </c>
       <c r="F35" s="18" t="n">
-        <v>0.9045801526717557</v>
+        <v>0.9085520745131245</v>
       </c>
       <c r="G35" s="18" t="n">
         <v>0.8630985915492958</v>
@@ -2046,7 +2032,7 @@
         <v>1154</v>
       </c>
       <c r="F36" s="17" t="n">
-        <v>0.914332784184514</v>
+        <v>0.8991452991452992</v>
       </c>
       <c r="G36" s="17" t="n">
         <v>0.8755411255411255</v>
@@ -2074,7 +2060,7 @@
         <v>1182</v>
       </c>
       <c r="F37" s="18" t="n">
-        <v>0.8371757925072046</v>
+        <v>0.7955706984667802</v>
       </c>
       <c r="G37" s="18" t="n">
         <v>0.8770999115826702</v>
@@ -2102,7 +2088,7 @@
         <v>448</v>
       </c>
       <c r="F38" s="17" t="n">
-        <v>0.6354929577464788</v>
+        <v>0.6071232876712329</v>
       </c>
       <c r="G38" s="17" t="n">
         <v>0.8386123680241327</v>
@@ -2188,7 +2174,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="18" t="n">
-        <v>0.8522727272727273</v>
+        <v>0.7438016528925619</v>
       </c>
       <c r="F44" s="18" t="n">
         <v>0.9026548672566371</v>
@@ -2209,10 +2195,8 @@
       <c r="D45" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="E45" s="17" t="inlineStr">
-        <is>
-          <t>غ/م</t>
-        </is>
+      <c r="E45" s="17" t="n">
+        <v>0.3809523809523809</v>
       </c>
       <c r="F45" s="17" t="n">
         <v>0.9607843137254902</v>
@@ -3264,15 +3248,17 @@
         <v>242</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="N14" s="14" t="n">
         <v>260</v>
       </c>
       <c r="O14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="18" t="n"/>
+        <v>99</v>
+      </c>
+      <c r="P14" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="Q14" s="18" t="n">
         <v>0.9730769230769231</v>
       </c>
@@ -3332,15 +3318,17 @@
         <v>68</v>
       </c>
       <c r="M15" s="11" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="N15" s="11" t="n">
         <v>63</v>
       </c>
       <c r="O15" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="17" t="n"/>
+        <v>260</v>
+      </c>
+      <c r="P15" s="17" t="n">
+        <v>0.9692307692307692</v>
+      </c>
       <c r="Q15" s="17" t="n">
         <v>0.9047619047619048</v>
       </c>
@@ -3400,16 +3388,16 @@
         <v>71</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="N16" s="14" t="n">
         <v>79</v>
       </c>
       <c r="O16" s="14" t="n">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="P16" s="18" t="n">
-        <v>1</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="Q16" s="18" t="n">
         <v>0.9367088607594937</v>
@@ -3470,16 +3458,16 @@
         <v>27</v>
       </c>
       <c r="M17" s="11" t="n">
-        <v>253</v>
+        <v>73</v>
       </c>
       <c r="N17" s="11" t="n">
         <v>28</v>
       </c>
       <c r="O17" s="11" t="n">
-        <v>260</v>
+        <v>79</v>
       </c>
       <c r="P17" s="17" t="n">
-        <v>0.9730769230769231</v>
+        <v>0.9240506329113924</v>
       </c>
       <c r="Q17" s="17" t="n">
         <v>0.9285714285714286</v>
@@ -3540,16 +3528,16 @@
         <v>3</v>
       </c>
       <c r="M18" s="14" t="n">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="N18" s="14" t="n">
         <v>42</v>
       </c>
       <c r="O18" s="14" t="n">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="P18" s="18" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="Q18" s="18" t="n">
         <v>0.8809523809523809</v>
@@ -4558,15 +4546,17 @@
         <v>4</v>
       </c>
       <c r="M33" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="11" t="n">
         <v>2</v>
       </c>
       <c r="O33" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" s="17" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="P33" s="17" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="Q33" s="17" t="n">
         <v>0.5</v>
       </c>
@@ -4626,15 +4616,17 @@
         <v>6</v>
       </c>
       <c r="M34" s="14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N34" s="14" t="n">
         <v>0</v>
       </c>
       <c r="O34" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" s="18" t="n"/>
+        <v>2</v>
+      </c>
+      <c r="P34" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="Q34" s="18" t="n"/>
       <c r="R34" s="18" t="n">
         <v>1</v>
@@ -4692,17 +4684,15 @@
         <v>7</v>
       </c>
       <c r="M35" s="11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N35" s="11" t="n">
         <v>6</v>
       </c>
       <c r="O35" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="P35" s="17" t="n">
-        <v>0.6666666666666666</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P35" s="17" t="n"/>
       <c r="Q35" s="17" t="n">
         <v>0.6666666666666666</v>
       </c>
@@ -4762,16 +4752,16 @@
         <v>4</v>
       </c>
       <c r="M36" s="14" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N36" s="14" t="n">
         <v>13</v>
       </c>
       <c r="O36" s="14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P36" s="18" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="Q36" s="18" t="n">
         <v>0.5384615384615384</v>
@@ -4832,15 +4822,17 @@
         <v>12</v>
       </c>
       <c r="M37" s="11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N37" s="11" t="n">
         <v>14</v>
       </c>
       <c r="O37" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="17" t="n"/>
+        <v>13</v>
+      </c>
+      <c r="P37" s="17" t="n">
+        <v>0.4615384615384616</v>
+      </c>
       <c r="Q37" s="17" t="n">
         <v>0.8571428571428571</v>
       </c>
@@ -4900,16 +4892,16 @@
         <v>1</v>
       </c>
       <c r="M38" s="14" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N38" s="14" t="n">
         <v>11</v>
       </c>
       <c r="O38" s="14" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="P38" s="18" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="Q38" s="18" t="n">
         <v>0.8181818181818182</v>
@@ -5172,15 +5164,17 @@
         <v>0</v>
       </c>
       <c r="M42" s="14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N42" s="14" t="n">
         <v>11</v>
       </c>
       <c r="O42" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" s="18" t="n"/>
+        <v>17</v>
+      </c>
+      <c r="P42" s="18" t="n">
+        <v>0.1176470588235294</v>
+      </c>
       <c r="Q42" s="18" t="n">
         <v>1</v>
       </c>
@@ -6326,9 +6320,11 @@
         <v>11</v>
       </c>
       <c r="O59" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P59" s="17" t="n"/>
+        <v>22</v>
+      </c>
+      <c r="P59" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="Q59" s="17" t="n">
         <v>0.9090909090909091</v>
       </c>
@@ -6394,9 +6390,11 @@
         <v>14</v>
       </c>
       <c r="O60" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P60" s="18" t="n"/>
+        <v>11</v>
+      </c>
+      <c r="P60" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="Q60" s="18" t="n">
         <v>0.9285714285714286</v>
       </c>
@@ -6656,15 +6654,17 @@
         <v>78</v>
       </c>
       <c r="M64" s="14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N64" s="14" t="n">
         <v>86</v>
       </c>
       <c r="O64" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P64" s="18" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="P64" s="18" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="Q64" s="18" t="n">
         <v>0.8488372093023255</v>
       </c>
@@ -6724,15 +6724,17 @@
         <v>197</v>
       </c>
       <c r="M65" s="11" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="N65" s="11" t="n">
         <v>230</v>
       </c>
       <c r="O65" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P65" s="17" t="n"/>
+        <v>86</v>
+      </c>
+      <c r="P65" s="17" t="n">
+        <v>0.8372093023255814</v>
+      </c>
       <c r="Q65" s="17" t="n">
         <v>0.908695652173913</v>
       </c>
@@ -6792,16 +6794,16 @@
         <v>58</v>
       </c>
       <c r="M66" s="14" t="n">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="N66" s="14" t="n">
         <v>55</v>
       </c>
       <c r="O66" s="14" t="n">
-        <v>3</v>
+        <v>230</v>
       </c>
       <c r="P66" s="18" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8608695652173913</v>
       </c>
       <c r="Q66" s="18" t="n">
         <v>0.7818181818181819</v>
@@ -6862,16 +6864,16 @@
         <v>65</v>
       </c>
       <c r="M67" s="11" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="N67" s="11" t="n">
         <v>68</v>
       </c>
       <c r="O67" s="11" t="n">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="P67" s="17" t="n">
-        <v>0.8372093023255814</v>
+        <v>0.8</v>
       </c>
       <c r="Q67" s="17" t="n">
         <v>0.7941176470588235</v>
@@ -6932,16 +6934,16 @@
         <v>29</v>
       </c>
       <c r="M68" s="14" t="n">
-        <v>206</v>
+        <v>54</v>
       </c>
       <c r="N68" s="14" t="n">
         <v>32</v>
       </c>
       <c r="O68" s="14" t="n">
-        <v>230</v>
+        <v>68</v>
       </c>
       <c r="P68" s="18" t="n">
-        <v>0.8956521739130435</v>
+        <v>0.7941176470588235</v>
       </c>
       <c r="Q68" s="18" t="n">
         <v>0.84375</v>
@@ -7002,16 +7004,16 @@
         <v>1</v>
       </c>
       <c r="M69" s="11" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="N69" s="11" t="n">
         <v>23</v>
       </c>
       <c r="O69" s="11" t="n">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="P69" s="17" t="n">
-        <v>0.8</v>
+        <v>0.71875</v>
       </c>
       <c r="Q69" s="17" t="n">
         <v>0.9565217391304348</v>
@@ -7274,15 +7276,17 @@
         <v>2</v>
       </c>
       <c r="M73" s="11" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N73" s="11" t="n">
         <v>13</v>
       </c>
       <c r="O73" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P73" s="17" t="n"/>
+        <v>28</v>
+      </c>
+      <c r="P73" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="Q73" s="17" t="n">
         <v>1</v>
       </c>
@@ -7476,15 +7480,17 @@
         <v>32</v>
       </c>
       <c r="M76" s="14" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="N76" s="14" t="n">
         <v>39</v>
       </c>
       <c r="O76" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P76" s="18" t="n"/>
+        <v>21</v>
+      </c>
+      <c r="P76" s="18" t="n">
+        <v>0.9047619047619048</v>
+      </c>
       <c r="Q76" s="18" t="n">
         <v>0.9487179487179487</v>
       </c>
@@ -7544,15 +7550,17 @@
         <v>28</v>
       </c>
       <c r="M77" s="11" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="N77" s="11" t="n">
         <v>28</v>
       </c>
       <c r="O77" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P77" s="17" t="n"/>
+        <v>39</v>
+      </c>
+      <c r="P77" s="17" t="n">
+        <v>0.9230769230769231</v>
+      </c>
       <c r="Q77" s="17" t="n">
         <v>0.8928571428571429</v>
       </c>
@@ -7612,16 +7620,16 @@
         <v>13</v>
       </c>
       <c r="M78" s="14" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N78" s="14" t="n">
         <v>11</v>
       </c>
       <c r="O78" s="14" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="P78" s="18" t="n">
-        <v>0.9523809523809523</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="Q78" s="18" t="n">
         <v>0.9090909090909091</v>
@@ -7682,16 +7690,16 @@
         <v>25</v>
       </c>
       <c r="M79" s="11" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="N79" s="11" t="n">
         <v>24</v>
       </c>
       <c r="O79" s="11" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="P79" s="17" t="n">
-        <v>0.9487179487179487</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="Q79" s="17" t="n">
         <v>0.875</v>
@@ -7752,16 +7760,16 @@
         <v>1</v>
       </c>
       <c r="M80" s="14" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N80" s="14" t="n">
         <v>9</v>
       </c>
       <c r="O80" s="14" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="P80" s="18" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="Q80" s="18" t="n">
         <v>0.8888888888888888</v>
@@ -8024,15 +8032,17 @@
         <v>0</v>
       </c>
       <c r="M84" s="14" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N84" s="14" t="n">
         <v>19</v>
       </c>
       <c r="O84" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P84" s="18" t="n"/>
+        <v>26</v>
+      </c>
+      <c r="P84" s="18" t="n">
+        <v>0.6923076923076923</v>
+      </c>
       <c r="Q84" s="18" t="n">
         <v>0.8947368421052632</v>
       </c>
@@ -8908,15 +8918,17 @@
         <v>5</v>
       </c>
       <c r="M97" s="11" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N97" s="11" t="n">
         <v>5</v>
       </c>
       <c r="O97" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P97" s="17" t="n"/>
+        <v>12</v>
+      </c>
+      <c r="P97" s="17" t="n">
+        <v>1</v>
+      </c>
       <c r="Q97" s="17" t="n">
         <v>1</v>
       </c>
@@ -8976,15 +8988,17 @@
         <v>17</v>
       </c>
       <c r="M98" s="14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N98" s="14" t="n">
         <v>24</v>
       </c>
       <c r="O98" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P98" s="18" t="n"/>
+        <v>5</v>
+      </c>
+      <c r="P98" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="Q98" s="18" t="n">
         <v>0.8333333333333334</v>
       </c>
@@ -9044,16 +9058,16 @@
         <v>14</v>
       </c>
       <c r="M99" s="11" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="N99" s="11" t="n">
         <v>20</v>
       </c>
       <c r="O99" s="11" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="P99" s="17" t="n">
-        <v>1</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="Q99" s="17" t="n">
         <v>0.8</v>
@@ -9114,16 +9128,16 @@
         <v>19</v>
       </c>
       <c r="M100" s="14" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="N100" s="14" t="n">
         <v>12</v>
       </c>
       <c r="O100" s="14" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P100" s="18" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Q100" s="18" t="n">
         <v>1</v>
@@ -9184,16 +9198,16 @@
         <v>0</v>
       </c>
       <c r="M101" s="11" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N101" s="11" t="n">
         <v>14</v>
       </c>
       <c r="O101" s="11" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="P101" s="17" t="n">
-        <v>0.7916666666666666</v>
+        <v>1</v>
       </c>
       <c r="Q101" s="17" t="n">
         <v>0.9285714285714286</v>
@@ -10072,15 +10086,17 @@
         <v>1</v>
       </c>
       <c r="M114" s="14" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N114" s="14" t="n">
         <v>8</v>
       </c>
       <c r="O114" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P114" s="18" t="n"/>
+        <v>34</v>
+      </c>
+      <c r="P114" s="18" t="n">
+        <v>0.3823529411764706</v>
+      </c>
       <c r="Q114" s="18" t="n">
         <v>1</v>
       </c>
@@ -10374,9 +10390,11 @@
         <v>1947</v>
       </c>
       <c r="K6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="18" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="L6" s="18" t="n">
+        <v>0.5</v>
+      </c>
       <c r="M6" s="18" t="n">
         <v>0.9579901153212521</v>
       </c>
@@ -10418,9 +10436,11 @@
         <v>1734</v>
       </c>
       <c r="K7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="17" t="n"/>
+        <v>204</v>
+      </c>
+      <c r="L7" s="17" t="n">
+        <v>0.9272727272727272</v>
+      </c>
       <c r="M7" s="17" t="n">
         <v>0.9313160422670509</v>
       </c>
@@ -10462,10 +10482,10 @@
         <v>1299</v>
       </c>
       <c r="K8" s="14" t="n">
-        <v>1659</v>
+        <v>2146</v>
       </c>
       <c r="L8" s="18" t="n">
-        <v>0.9045801526717557</v>
+        <v>0.9085520745131245</v>
       </c>
       <c r="M8" s="18" t="n">
         <v>0.8630985915492958</v>
@@ -10508,10 +10528,10 @@
         <v>1154</v>
       </c>
       <c r="K9" s="11" t="n">
-        <v>1110</v>
+        <v>1052</v>
       </c>
       <c r="L9" s="17" t="n">
-        <v>0.914332784184514</v>
+        <v>0.8991452991452992</v>
       </c>
       <c r="M9" s="17" t="n">
         <v>0.8755411255411255</v>
@@ -10554,10 +10574,10 @@
         <v>1182</v>
       </c>
       <c r="K10" s="14" t="n">
-        <v>1743</v>
+        <v>1401</v>
       </c>
       <c r="L10" s="18" t="n">
-        <v>0.8371757925072046</v>
+        <v>0.7955706984667802</v>
       </c>
       <c r="M10" s="18" t="n">
         <v>0.8770999115826702</v>
@@ -10600,10 +10620,10 @@
         <v>448</v>
       </c>
       <c r="K11" s="11" t="n">
-        <v>1128</v>
+        <v>1108</v>
       </c>
       <c r="L11" s="17" t="n">
-        <v>0.6354929577464788</v>
+        <v>0.6071232876712329</v>
       </c>
       <c r="M11" s="17" t="n">
         <v>0.8386123680241327</v>
@@ -10846,10 +10866,10 @@
         <v>3</v>
       </c>
       <c r="M4" s="14" t="n">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="N4" s="18" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="O4" s="18" t="n">
         <v>0.8809523809523809</v>
@@ -10962,10 +10982,10 @@
         <v>1</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N6" s="18" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="O6" s="18" t="n">
         <v>0.8181818181818182</v>
@@ -11020,9 +11040,11 @@
         <v>0</v>
       </c>
       <c r="M7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="17" t="n"/>
+        <v>2</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>0.1176470588235294</v>
+      </c>
       <c r="O7" s="17" t="n">
         <v>1</v>
       </c>
@@ -11136,7 +11158,9 @@
       <c r="M9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="N9" s="17" t="n"/>
+      <c r="N9" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="O9" s="17" t="n">
         <v>0.9285714285714286</v>
       </c>
@@ -11190,10 +11214,10 @@
         <v>1</v>
       </c>
       <c r="M10" s="14" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="N10" s="18" t="n">
-        <v>0.8</v>
+        <v>0.71875</v>
       </c>
       <c r="O10" s="18" t="n">
         <v>0.9565217391304348</v>
@@ -11248,9 +11272,11 @@
         <v>2</v>
       </c>
       <c r="M11" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="17" t="n"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="O11" s="17" t="n">
         <v>1</v>
       </c>
@@ -11358,9 +11384,11 @@
         <v>0</v>
       </c>
       <c r="M13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" s="17" t="n"/>
+        <v>18</v>
+      </c>
+      <c r="N13" s="17" t="n">
+        <v>0.6923076923076923</v>
+      </c>
       <c r="O13" s="17" t="n">
         <v>0.8947368421052632</v>
       </c>
@@ -11414,10 +11442,10 @@
         <v>1</v>
       </c>
       <c r="M14" s="14" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N14" s="18" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="O14" s="18" t="n">
         <v>0.8888888888888888</v>
@@ -11530,10 +11558,10 @@
         <v>0</v>
       </c>
       <c r="M16" s="14" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N16" s="18" t="n">
-        <v>0.7916666666666666</v>
+        <v>1</v>
       </c>
       <c r="O16" s="18" t="n">
         <v>0.9285714285714286</v>
@@ -11646,9 +11674,11 @@
         <v>1</v>
       </c>
       <c r="M18" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="18" t="n"/>
+        <v>13</v>
+      </c>
+      <c r="N18" s="18" t="n">
+        <v>0.3823529411764706</v>
+      </c>
       <c r="O18" s="18" t="n">
         <v>1</v>
       </c>
@@ -12877,15 +12907,17 @@
         <v>242</v>
       </c>
       <c r="H13" s="11" t="n">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I13" s="11" t="n">
         <v>260</v>
       </c>
       <c r="J13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="17" t="inlineStr"/>
+        <v>99</v>
+      </c>
+      <c r="K13" s="17" t="n">
+        <v>1</v>
+      </c>
       <c r="L13" s="17" t="n">
         <v>0.9730769230769231</v>
       </c>
@@ -12919,15 +12951,17 @@
         <v>68</v>
       </c>
       <c r="H14" s="14" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="I14" s="14" t="n">
         <v>63</v>
       </c>
       <c r="J14" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="18" t="inlineStr"/>
+        <v>260</v>
+      </c>
+      <c r="K14" s="18" t="n">
+        <v>0.9692307692307692</v>
+      </c>
       <c r="L14" s="18" t="n">
         <v>0.9047619047619048</v>
       </c>
@@ -12961,16 +12995,16 @@
         <v>71</v>
       </c>
       <c r="H15" s="11" t="n">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="I15" s="11" t="n">
         <v>79</v>
       </c>
       <c r="J15" s="11" t="n">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="K15" s="17" t="n">
-        <v>1</v>
+        <v>0.9047619047619048</v>
       </c>
       <c r="L15" s="17" t="n">
         <v>0.9367088607594937</v>
@@ -13005,16 +13039,16 @@
         <v>27</v>
       </c>
       <c r="H16" s="14" t="n">
-        <v>253</v>
+        <v>73</v>
       </c>
       <c r="I16" s="14" t="n">
         <v>28</v>
       </c>
       <c r="J16" s="14" t="n">
-        <v>260</v>
+        <v>79</v>
       </c>
       <c r="K16" s="18" t="n">
-        <v>0.9730769230769231</v>
+        <v>0.9240506329113924</v>
       </c>
       <c r="L16" s="18" t="n">
         <v>0.9285714285714286</v>
@@ -13049,16 +13083,16 @@
         <v>3</v>
       </c>
       <c r="H17" s="11" t="n">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="I17" s="11" t="n">
         <v>42</v>
       </c>
       <c r="J17" s="11" t="n">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="K17" s="17" t="n">
-        <v>0.9047619047619048</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="L17" s="17" t="n">
         <v>0.8809523809523809</v>
@@ -13517,15 +13551,17 @@
         <v>4</v>
       </c>
       <c r="H28" s="14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="14" t="n">
         <v>2</v>
       </c>
       <c r="J28" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="18" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="K28" s="18" t="n">
+        <v>0.3333333333333333</v>
+      </c>
       <c r="L28" s="18" t="n">
         <v>0.5</v>
       </c>
@@ -13559,15 +13595,17 @@
         <v>6</v>
       </c>
       <c r="H29" s="11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" s="11" t="n">
         <v>0</v>
       </c>
       <c r="J29" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="17" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="K29" s="17" t="n">
+        <v>1</v>
+      </c>
       <c r="L29" s="17" t="inlineStr"/>
     </row>
     <row r="30">
@@ -13599,17 +13637,15 @@
         <v>7</v>
       </c>
       <c r="H30" s="14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I30" s="14" t="n">
         <v>6</v>
       </c>
       <c r="J30" s="14" t="n">
-        <v>3</v>
-      </c>
-      <c r="K30" s="18" t="n">
-        <v>0.6666666666666666</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K30" s="18" t="inlineStr"/>
       <c r="L30" s="18" t="n">
         <v>0.6666666666666666</v>
       </c>
@@ -13643,16 +13679,16 @@
         <v>4</v>
       </c>
       <c r="H31" s="11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I31" s="11" t="n">
         <v>13</v>
       </c>
       <c r="J31" s="11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K31" s="17" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="L31" s="17" t="n">
         <v>0.5384615384615384</v>
@@ -13687,15 +13723,17 @@
         <v>12</v>
       </c>
       <c r="H32" s="14" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I32" s="14" t="n">
         <v>14</v>
       </c>
       <c r="J32" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="18" t="inlineStr"/>
+        <v>13</v>
+      </c>
+      <c r="K32" s="18" t="n">
+        <v>0.4615384615384616</v>
+      </c>
       <c r="L32" s="18" t="n">
         <v>0.8571428571428571</v>
       </c>
@@ -13729,16 +13767,16 @@
         <v>1</v>
       </c>
       <c r="H33" s="11" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I33" s="11" t="n">
         <v>11</v>
       </c>
       <c r="J33" s="11" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K33" s="17" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="L33" s="17" t="n">
         <v>0.8181818181818182</v>
@@ -13897,15 +13935,17 @@
         <v>0</v>
       </c>
       <c r="H37" s="11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" s="11" t="n">
         <v>11</v>
       </c>
       <c r="J37" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" s="17" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="K37" s="17" t="n">
+        <v>0.1176470588235294</v>
+      </c>
       <c r="L37" s="17" t="n">
         <v>1</v>
       </c>
@@ -14529,9 +14569,11 @@
         <v>11</v>
       </c>
       <c r="J52" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K52" s="18" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="K52" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="L52" s="18" t="n">
         <v>0.9090909090909091</v>
       </c>
@@ -14571,9 +14613,11 @@
         <v>14</v>
       </c>
       <c r="J53" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K53" s="17" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="K53" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="L53" s="17" t="n">
         <v>0.9285714285714286</v>
       </c>
@@ -14689,15 +14733,17 @@
         <v>78</v>
       </c>
       <c r="H56" s="14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I56" s="14" t="n">
         <v>86</v>
       </c>
       <c r="J56" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" s="18" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="K56" s="18" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="L56" s="18" t="n">
         <v>0.8488372093023255</v>
       </c>
@@ -14731,15 +14777,17 @@
         <v>197</v>
       </c>
       <c r="H57" s="11" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="I57" s="11" t="n">
         <v>230</v>
       </c>
       <c r="J57" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" s="17" t="inlineStr"/>
+        <v>86</v>
+      </c>
+      <c r="K57" s="17" t="n">
+        <v>0.8372093023255814</v>
+      </c>
       <c r="L57" s="17" t="n">
         <v>0.908695652173913</v>
       </c>
@@ -14773,16 +14821,16 @@
         <v>58</v>
       </c>
       <c r="H58" s="14" t="n">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="I58" s="14" t="n">
         <v>55</v>
       </c>
       <c r="J58" s="14" t="n">
-        <v>3</v>
+        <v>230</v>
       </c>
       <c r="K58" s="18" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8608695652173913</v>
       </c>
       <c r="L58" s="18" t="n">
         <v>0.7818181818181819</v>
@@ -14817,16 +14865,16 @@
         <v>65</v>
       </c>
       <c r="H59" s="11" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="I59" s="11" t="n">
         <v>68</v>
       </c>
       <c r="J59" s="11" t="n">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="K59" s="17" t="n">
-        <v>0.8372093023255814</v>
+        <v>0.8</v>
       </c>
       <c r="L59" s="17" t="n">
         <v>0.7941176470588235</v>
@@ -14861,16 +14909,16 @@
         <v>29</v>
       </c>
       <c r="H60" s="14" t="n">
-        <v>206</v>
+        <v>54</v>
       </c>
       <c r="I60" s="14" t="n">
         <v>32</v>
       </c>
       <c r="J60" s="14" t="n">
-        <v>230</v>
+        <v>68</v>
       </c>
       <c r="K60" s="18" t="n">
-        <v>0.8956521739130435</v>
+        <v>0.7941176470588235</v>
       </c>
       <c r="L60" s="18" t="n">
         <v>0.84375</v>
@@ -14905,16 +14953,16 @@
         <v>1</v>
       </c>
       <c r="H61" s="11" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="I61" s="11" t="n">
         <v>23</v>
       </c>
       <c r="J61" s="11" t="n">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="K61" s="17" t="n">
-        <v>0.8</v>
+        <v>0.71875</v>
       </c>
       <c r="L61" s="17" t="n">
         <v>0.9565217391304348</v>
@@ -15073,15 +15121,17 @@
         <v>2</v>
       </c>
       <c r="H65" s="11" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I65" s="11" t="n">
         <v>13</v>
       </c>
       <c r="J65" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K65" s="17" t="inlineStr"/>
+        <v>28</v>
+      </c>
+      <c r="K65" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="L65" s="17" t="n">
         <v>1</v>
       </c>
@@ -15319,15 +15369,17 @@
         <v>0</v>
       </c>
       <c r="H71" s="11" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I71" s="11" t="n">
         <v>19</v>
       </c>
       <c r="J71" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K71" s="17" t="inlineStr"/>
+        <v>26</v>
+      </c>
+      <c r="K71" s="17" t="n">
+        <v>0.6923076923076923</v>
+      </c>
       <c r="L71" s="17" t="n">
         <v>0.8947368421052632</v>
       </c>
@@ -15443,15 +15495,17 @@
         <v>32</v>
       </c>
       <c r="H74" s="14" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I74" s="14" t="n">
         <v>39</v>
       </c>
       <c r="J74" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K74" s="18" t="inlineStr"/>
+        <v>21</v>
+      </c>
+      <c r="K74" s="18" t="n">
+        <v>0.9047619047619048</v>
+      </c>
       <c r="L74" s="18" t="n">
         <v>0.9487179487179487</v>
       </c>
@@ -15485,15 +15539,17 @@
         <v>28</v>
       </c>
       <c r="H75" s="11" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I75" s="11" t="n">
         <v>28</v>
       </c>
       <c r="J75" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K75" s="17" t="inlineStr"/>
+        <v>39</v>
+      </c>
+      <c r="K75" s="17" t="n">
+        <v>0.9230769230769231</v>
+      </c>
       <c r="L75" s="17" t="n">
         <v>0.8928571428571429</v>
       </c>
@@ -15527,16 +15583,16 @@
         <v>13</v>
       </c>
       <c r="H76" s="14" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I76" s="14" t="n">
         <v>11</v>
       </c>
       <c r="J76" s="14" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="K76" s="18" t="n">
-        <v>0.9523809523809523</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="L76" s="18" t="n">
         <v>0.9090909090909091</v>
@@ -15571,16 +15627,16 @@
         <v>25</v>
       </c>
       <c r="H77" s="11" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="I77" s="11" t="n">
         <v>24</v>
       </c>
       <c r="J77" s="11" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="K77" s="17" t="n">
-        <v>0.9487179487179487</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="L77" s="17" t="n">
         <v>0.875</v>
@@ -15615,16 +15671,16 @@
         <v>1</v>
       </c>
       <c r="H78" s="14" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I78" s="14" t="n">
         <v>9</v>
       </c>
       <c r="J78" s="14" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K78" s="18" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="L78" s="18" t="n">
         <v>0.8888888888888888</v>
@@ -16123,15 +16179,17 @@
         <v>5</v>
       </c>
       <c r="H90" s="14" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I90" s="14" t="n">
         <v>5</v>
       </c>
       <c r="J90" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K90" s="18" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="K90" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="L90" s="18" t="n">
         <v>1</v>
       </c>
@@ -16165,15 +16223,17 @@
         <v>17</v>
       </c>
       <c r="H91" s="11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I91" s="11" t="n">
         <v>24</v>
       </c>
       <c r="J91" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K91" s="17" t="inlineStr"/>
+        <v>5</v>
+      </c>
+      <c r="K91" s="17" t="n">
+        <v>1</v>
+      </c>
       <c r="L91" s="17" t="n">
         <v>0.8333333333333334</v>
       </c>
@@ -16207,16 +16267,16 @@
         <v>14</v>
       </c>
       <c r="H92" s="14" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I92" s="14" t="n">
         <v>20</v>
       </c>
       <c r="J92" s="14" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K92" s="18" t="n">
-        <v>1</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="L92" s="18" t="n">
         <v>0.8</v>
@@ -16251,16 +16311,16 @@
         <v>19</v>
       </c>
       <c r="H93" s="11" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I93" s="11" t="n">
         <v>12</v>
       </c>
       <c r="J93" s="11" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K93" s="17" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L93" s="17" t="n">
         <v>1</v>
@@ -16295,16 +16355,16 @@
         <v>0</v>
       </c>
       <c r="H94" s="14" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I94" s="14" t="n">
         <v>14</v>
       </c>
       <c r="J94" s="14" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K94" s="18" t="n">
-        <v>0.7916666666666666</v>
+        <v>1</v>
       </c>
       <c r="L94" s="18" t="n">
         <v>0.9285714285714286</v>
@@ -16805,15 +16865,17 @@
         <v>1</v>
       </c>
       <c r="H106" s="14" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I106" s="14" t="n">
         <v>8</v>
       </c>
       <c r="J106" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K106" s="18" t="inlineStr"/>
+        <v>34</v>
+      </c>
+      <c r="K106" s="18" t="n">
+        <v>0.3823529411764706</v>
+      </c>
       <c r="L106" s="18" t="n">
         <v>1</v>
       </c>

</xml_diff>